<commit_message>
chore: update Norfolk coastal flooding benchmark datachore: update Norfolk coastal flooding benchmark data
</commit_message>
<xml_diff>
--- a/test_data/norfolk_coastal_flooding/full_benchmarking_experiment_frontier.xlsx
+++ b/test_data/norfolk_coastal_flooding/full_benchmarking_experiment_frontier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dcl3nd\dev\TRITON-SWMM_toolkit\test_data\norfolk_coastal_flooding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912B56BB-603B-4FDB-8F8B-A6C2D068F3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD7A665-DA51-4046-8220-8702735846D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4185" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="22">
   <si>
     <t>CPU</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>gpu</t>
+  </si>
+  <si>
+    <t>check</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -393,6 +396,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -400,7 +405,10 @@
     <cellStyle name="Note" xfId="3" builtinId="10"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -694,16 +702,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -718,8 +726,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12706350" y="104775"/>
-          <a:ext cx="4276725" cy="2247899"/>
+          <a:off x="17602200" y="0"/>
+          <a:ext cx="4276725" cy="2762250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -830,24 +838,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}" name="Table1" displayName="Table1" ref="A1:J55" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:J55" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}"/>
-  <tableColumns count="10">
-    <tableColumn id="11" xr3:uid="{3DECB62C-AAF2-4EC7-8598-5E8776D4B845}" name="hardware_utilization_strategy" dataDxfId="9" dataCellStyle="Note"/>
-    <tableColumn id="9" xr3:uid="{047B8296-C28F-43DA-A753-CC6445B34CE4}" name="device" dataDxfId="8" dataCellStyle="Note"/>
-    <tableColumn id="1" xr3:uid="{16000747-EB63-4EDF-971B-D9460636B6A5}" name="run_mode" dataDxfId="7" dataCellStyle="Input"/>
-    <tableColumn id="2" xr3:uid="{09DC1F4B-B2B0-493A-B83E-1D7D4EA31F4C}" name="n_nodes" dataDxfId="6" dataCellStyle="Input"/>
-    <tableColumn id="3" xr3:uid="{3A65E5E5-CB8B-4698-A27C-21DF3A95D49A}" name="n_mpi_procs" dataDxfId="5" dataCellStyle="Input"/>
-    <tableColumn id="4" xr3:uid="{D366E835-7967-45B3-94DD-92B04C3126AA}" name="n_omp_threads" dataDxfId="4" dataCellStyle="Input"/>
-    <tableColumn id="8" xr3:uid="{53D9FE6F-92F7-4A3A-B94F-6A698F029BE0}" name="n_gpus" dataDxfId="3" dataCellStyle="Input"/>
-    <tableColumn id="6" xr3:uid="{F6B7A6B4-BD4B-4406-BCB7-C3DBCC48FA6B}" name="total_OpenMP_threads" dataDxfId="2" dataCellStyle="Output">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}" name="Table1" displayName="Table1" ref="A1:K54" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K54" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K54">
+    <sortCondition ref="C1:C54"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="11" xr3:uid="{3DECB62C-AAF2-4EC7-8598-5E8776D4B845}" name="hardware_utilization_strategy" dataDxfId="10" dataCellStyle="Note"/>
+    <tableColumn id="9" xr3:uid="{047B8296-C28F-43DA-A753-CC6445B34CE4}" name="device" dataDxfId="9" dataCellStyle="Note"/>
+    <tableColumn id="1" xr3:uid="{16000747-EB63-4EDF-971B-D9460636B6A5}" name="run_mode" dataDxfId="8" dataCellStyle="Input"/>
+    <tableColumn id="2" xr3:uid="{09DC1F4B-B2B0-493A-B83E-1D7D4EA31F4C}" name="n_nodes" dataDxfId="7" dataCellStyle="Input"/>
+    <tableColumn id="3" xr3:uid="{3A65E5E5-CB8B-4698-A27C-21DF3A95D49A}" name="n_mpi_procs" dataDxfId="6" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{D366E835-7967-45B3-94DD-92B04C3126AA}" name="n_omp_threads" dataDxfId="5" dataCellStyle="Input"/>
+    <tableColumn id="8" xr3:uid="{53D9FE6F-92F7-4A3A-B94F-6A698F029BE0}" name="n_gpus" dataDxfId="4" dataCellStyle="Input"/>
+    <tableColumn id="6" xr3:uid="{F6B7A6B4-BD4B-4406-BCB7-C3DBCC48FA6B}" name="total_OpenMP_threads" dataDxfId="3" dataCellStyle="Output">
       <calculatedColumnFormula>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8B064801-C992-4C19-AF9B-73CC7D0951B1}" name="total_devices" dataDxfId="1" dataCellStyle="Output">
+    <tableColumn id="7" xr3:uid="{8B064801-C992-4C19-AF9B-73CC7D0951B1}" name="total_devices" dataDxfId="2" dataCellStyle="Output">
       <calculatedColumnFormula>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C813D3D6-6AEA-4168-A5C0-6FD56BB1D36D}" name="devices_per_node" dataDxfId="0" dataCellStyle="Output">
+    <tableColumn id="10" xr3:uid="{C813D3D6-6AEA-4168-A5C0-6FD56BB1D36D}" name="devices_per_node" dataDxfId="1" dataCellStyle="Output">
       <calculatedColumnFormula>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{47E652A1-51DD-4A45-9FB0-F72E592EF0D3}" name="check" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1117,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,7 +1151,7 @@
     <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1168,8 +1182,11 @@
       <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1203,8 +1220,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1238,8 +1259,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1273,8 +1298,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1308,8 +1337,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1343,8 +1376,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
@@ -1378,8 +1415,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1413,8 +1454,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
@@ -1448,113 +1493,129 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="14" t="s">
+      <c r="K9" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6">
         <v>16</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
+      <c r="F10" s="6">
         <v>1</v>
       </c>
       <c r="G10" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H10" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I10" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J10" s="8">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="14">
-        <v>1</v>
-      </c>
-      <c r="E11" s="14">
-        <v>2</v>
-      </c>
-      <c r="F11" s="14">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="K10" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6">
+        <v>32</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
       </c>
       <c r="G11" s="6">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H11" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="I11" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="J11" s="8">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="15">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14">
-        <v>2</v>
-      </c>
-      <c r="F12" s="15">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="K11" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="9">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6">
+        <v>64</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
       </c>
       <c r="G12" s="6">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="H12" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="I12" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="J12" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
@@ -1568,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13" s="14">
         <v>2</v>
@@ -1578,18 +1639,22 @@
       </c>
       <c r="H13" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I13" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J13" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="K13" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>5</v>
       </c>
@@ -1603,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F14" s="14">
         <v>4</v>
@@ -1613,18 +1678,22 @@
       </c>
       <c r="H14" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I14" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J14" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="K14" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>5</v>
       </c>
@@ -1638,28 +1707,32 @@
         <v>1</v>
       </c>
       <c r="E15" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F15" s="14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G15" s="6">
         <v>0</v>
       </c>
       <c r="H15" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I15" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J15" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="K15" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
@@ -1673,10 +1746,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F16" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G16" s="6">
         <v>0</v>
@@ -1693,8 +1766,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>5</v>
       </c>
@@ -1708,28 +1785,32 @@
         <v>1</v>
       </c>
       <c r="E17" s="14">
+        <v>2</v>
+      </c>
+      <c r="F17" s="14">
+        <v>8</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
         <v>16</v>
       </c>
-      <c r="F17" s="14">
-        <v>2</v>
-      </c>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
-      <c r="H17" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>32</v>
-      </c>
       <c r="I17" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="J17" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="K17" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>5</v>
       </c>
@@ -1743,28 +1824,32 @@
         <v>1</v>
       </c>
       <c r="E18" s="14">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F18" s="14">
+        <v>2</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
         <v>16</v>
       </c>
-      <c r="G18" s="6">
-        <v>0</v>
-      </c>
-      <c r="H18" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>32</v>
-      </c>
       <c r="I18" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="J18" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="K18" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>5</v>
       </c>
@@ -1778,10 +1863,10 @@
         <v>1</v>
       </c>
       <c r="E19" s="14">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F19" s="14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G19" s="6">
         <v>0</v>
@@ -1798,8 +1883,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>5</v>
       </c>
@@ -1813,10 +1902,10 @@
         <v>1</v>
       </c>
       <c r="E20" s="14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F20" s="14">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G20" s="6">
         <v>0</v>
@@ -1833,8 +1922,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>5</v>
       </c>
@@ -1848,28 +1941,32 @@
         <v>1</v>
       </c>
       <c r="E21" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F21" s="14">
+        <v>8</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
         <v>32</v>
       </c>
-      <c r="G21" s="6">
-        <v>0</v>
-      </c>
-      <c r="H21" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>64</v>
-      </c>
       <c r="I21" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="J21" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="K21" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>5</v>
       </c>
@@ -1883,28 +1980,32 @@
         <v>1</v>
       </c>
       <c r="E22" s="14">
+        <v>8</v>
+      </c>
+      <c r="F22" s="14">
+        <v>4</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
         <v>32</v>
       </c>
-      <c r="F22" s="14">
-        <v>2</v>
-      </c>
-      <c r="G22" s="6">
-        <v>0</v>
-      </c>
-      <c r="H22" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>64</v>
-      </c>
       <c r="I22" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="J22" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="K22" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>5</v>
       </c>
@@ -1918,10 +2019,10 @@
         <v>1</v>
       </c>
       <c r="E23" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F23" s="14">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G23" s="6">
         <v>0</v>
@@ -1938,8 +2039,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>5</v>
       </c>
@@ -1953,10 +2058,10 @@
         <v>1</v>
       </c>
       <c r="E24" s="14">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F24" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G24" s="6">
         <v>0</v>
@@ -1973,8 +2078,12 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>5</v>
       </c>
@@ -1988,10 +2097,10 @@
         <v>1</v>
       </c>
       <c r="E25" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F25" s="14">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G25" s="6">
         <v>0</v>
@@ -2008,463 +2117,519 @@
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="14">
         <v>1</v>
       </c>
       <c r="E26" s="14">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F26" s="14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G26" s="6">
         <v>0</v>
       </c>
       <c r="H26" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="I26" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="J26" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K26" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="14">
         <v>1</v>
       </c>
       <c r="E27" s="14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F27" s="14">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G27" s="6">
         <v>0</v>
       </c>
       <c r="H27" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="I27" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="J27" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K27" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="14">
-        <v>1</v>
-      </c>
-      <c r="E28" s="14">
-        <v>8</v>
-      </c>
-      <c r="F28" s="14">
-        <v>1</v>
-      </c>
-      <c r="G28" s="6">
+        <v>17</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2</v>
+      </c>
+      <c r="E28" s="6">
+        <v>2</v>
+      </c>
+      <c r="F28" s="6">
+        <v>64</v>
+      </c>
+      <c r="G28" s="20">
         <v>0</v>
       </c>
       <c r="H28" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="I28" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="J28" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K28" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="14">
+        <v>4</v>
+      </c>
+      <c r="F29" s="14">
+        <v>32</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0</v>
+      </c>
+      <c r="H29" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>128</v>
+      </c>
+      <c r="I29" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>128</v>
+      </c>
+      <c r="J29" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K29" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="14">
+        <v>2</v>
+      </c>
+      <c r="E30" s="14">
+        <v>8</v>
+      </c>
+      <c r="F30" s="14">
         <v>16</v>
       </c>
-      <c r="F29" s="14">
-        <v>1</v>
-      </c>
-      <c r="G29" s="6">
-        <v>0</v>
-      </c>
-      <c r="H29" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+      <c r="G30" s="6">
+        <v>0</v>
+      </c>
+      <c r="H30" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>128</v>
+      </c>
+      <c r="I30" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>128</v>
+      </c>
+      <c r="J30" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K30" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="14">
+        <v>2</v>
+      </c>
+      <c r="E31" s="14">
         <v>16</v>
       </c>
-      <c r="I29" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+      <c r="F31" s="14">
+        <v>8</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0</v>
+      </c>
+      <c r="H31" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>128</v>
+      </c>
+      <c r="I31" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>128</v>
+      </c>
+      <c r="J31" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K31" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="14">
+        <v>2</v>
+      </c>
+      <c r="E32" s="14">
+        <v>32</v>
+      </c>
+      <c r="F32" s="14">
+        <v>4</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>128</v>
+      </c>
+      <c r="I32" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>128</v>
+      </c>
+      <c r="J32" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K32" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="14">
+        <v>2</v>
+      </c>
+      <c r="E33" s="6">
+        <v>64</v>
+      </c>
+      <c r="F33" s="6">
+        <v>2</v>
+      </c>
+      <c r="G33" s="20">
+        <v>0</v>
+      </c>
+      <c r="H33" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>128</v>
+      </c>
+      <c r="I33" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>128</v>
+      </c>
+      <c r="J33" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K33" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="14">
+        <v>4</v>
+      </c>
+      <c r="E34" s="14">
         <v>16</v>
       </c>
-      <c r="J29" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+      <c r="F34" s="14">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="14">
-        <v>1</v>
-      </c>
-      <c r="E30" s="14">
+      <c r="G34" s="6">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>256</v>
+      </c>
+      <c r="I34" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>256</v>
+      </c>
+      <c r="J34" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K34" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="14">
+        <v>4</v>
+      </c>
+      <c r="E35" s="14">
+        <v>8</v>
+      </c>
+      <c r="F35" s="14">
         <v>32</v>
       </c>
-      <c r="F30" s="14">
-        <v>1</v>
-      </c>
-      <c r="G30" s="6">
-        <v>0</v>
-      </c>
-      <c r="H30" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+      <c r="G35" s="6">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>256</v>
+      </c>
+      <c r="I35" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>256</v>
+      </c>
+      <c r="J35" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K35" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="14">
+        <v>4</v>
+      </c>
+      <c r="E36" s="14">
+        <v>4</v>
+      </c>
+      <c r="F36" s="14">
+        <v>64</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>256</v>
+      </c>
+      <c r="I36" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>256</v>
+      </c>
+      <c r="J36" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K36" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="14">
+        <v>4</v>
+      </c>
+      <c r="E37" s="6">
         <v>32</v>
       </c>
-      <c r="I30" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>32</v>
-      </c>
-      <c r="J30" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="14">
-        <v>1</v>
-      </c>
-      <c r="E31" s="14">
-        <v>64</v>
-      </c>
-      <c r="F31" s="14">
-        <v>1</v>
-      </c>
-      <c r="G31" s="6">
-        <v>0</v>
-      </c>
-      <c r="H31" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>64</v>
-      </c>
-      <c r="I31" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>64</v>
-      </c>
-      <c r="J31" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="14">
-        <v>1</v>
-      </c>
-      <c r="E32" s="14">
-        <v>1</v>
-      </c>
-      <c r="F32" s="14">
-        <v>2</v>
-      </c>
-      <c r="G32" s="6">
-        <v>0</v>
-      </c>
-      <c r="H32" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>2</v>
-      </c>
-      <c r="I32" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>2</v>
-      </c>
-      <c r="J32" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="14">
-        <v>1</v>
-      </c>
-      <c r="E33" s="14">
-        <v>1</v>
-      </c>
-      <c r="F33" s="14">
-        <v>4</v>
-      </c>
-      <c r="G33" s="6">
-        <v>0</v>
-      </c>
-      <c r="H33" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>4</v>
-      </c>
-      <c r="I33" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>4</v>
-      </c>
-      <c r="J33" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="14">
-        <v>1</v>
-      </c>
-      <c r="E34" s="14">
-        <v>1</v>
-      </c>
-      <c r="F34" s="14">
-        <v>8</v>
-      </c>
-      <c r="G34" s="6">
-        <v>0</v>
-      </c>
-      <c r="H34" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>8</v>
-      </c>
-      <c r="I34" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>8</v>
-      </c>
-      <c r="J34" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="14">
-        <v>1</v>
-      </c>
-      <c r="E35" s="14">
-        <v>1</v>
-      </c>
-      <c r="F35" s="14">
-        <v>16</v>
-      </c>
-      <c r="G35" s="6">
-        <v>0</v>
-      </c>
-      <c r="H35" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>16</v>
-      </c>
-      <c r="I35" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>16</v>
-      </c>
-      <c r="J35" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="14">
-        <v>1</v>
-      </c>
-      <c r="E36" s="14">
-        <v>1</v>
-      </c>
-      <c r="F36" s="14">
-        <v>32</v>
-      </c>
-      <c r="G36" s="6">
-        <v>0</v>
-      </c>
-      <c r="H36" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>32</v>
-      </c>
-      <c r="I36" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>32</v>
-      </c>
-      <c r="J36" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="14">
-        <v>1</v>
-      </c>
-      <c r="E37" s="14">
-        <v>1</v>
-      </c>
-      <c r="F37" s="14">
-        <v>64</v>
+      <c r="F37" s="6">
+        <v>8</v>
       </c>
       <c r="G37" s="6">
         <v>0</v>
       </c>
       <c r="H37" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="I37" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="J37" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="6">
-        <v>2</v>
+      <c r="K37" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="14">
+        <v>4</v>
       </c>
       <c r="E38" s="6">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="F38" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G38" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H38" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>16</v>
+        <v>256</v>
       </c>
       <c r="I38" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>16</v>
+        <v>256</v>
       </c>
       <c r="J38" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K38" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>5</v>
       </c>
@@ -2474,137 +2639,153 @@
       <c r="C39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="6">
-        <v>2</v>
+      <c r="D39" s="14">
+        <v>4</v>
       </c>
       <c r="E39" s="6">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F39" s="6">
-        <v>64</v>
-      </c>
-      <c r="G39" s="20">
+        <v>2</v>
+      </c>
+      <c r="G39" s="6">
         <v>0</v>
       </c>
       <c r="H39" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="I39" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J39" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D40" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F40" s="14">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="G40" s="6">
         <v>0</v>
       </c>
       <c r="H40" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="I40" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="J40" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K40" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D41" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F41" s="14">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G41" s="6">
         <v>0</v>
       </c>
       <c r="H41" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="I41" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="J41" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="K41" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B42" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D42" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" s="14">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F42" s="14">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G42" s="6">
         <v>0</v>
       </c>
       <c r="H42" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="I42" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="J42" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="K42" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>4</v>
       </c>
@@ -2615,10 +2796,10 @@
         <v>18</v>
       </c>
       <c r="D43" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" s="14">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="F43" s="14">
         <v>1</v>
@@ -2628,435 +2809,448 @@
       </c>
       <c r="H43" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="I43" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="J43" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="K43" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D44" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44" s="14">
         <v>32</v>
       </c>
       <c r="F44" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G44" s="6">
         <v>0</v>
       </c>
       <c r="H44" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>32</v>
+      </c>
+      <c r="I44" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>32</v>
+      </c>
+      <c r="J44" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="K44" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="14">
+        <v>1</v>
+      </c>
+      <c r="E45" s="14">
+        <v>64</v>
+      </c>
+      <c r="F45" s="14">
+        <v>1</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0</v>
+      </c>
+      <c r="H45" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>64</v>
+      </c>
+      <c r="I45" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>64</v>
+      </c>
+      <c r="J45" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K45" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="14">
+        <v>2</v>
+      </c>
+      <c r="E46" s="14">
         <v>128</v>
       </c>
-      <c r="I44" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+      <c r="F46" s="14">
+        <v>1</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0</v>
+      </c>
+      <c r="H46" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
         <v>128</v>
       </c>
-      <c r="J44" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="14">
-        <v>2</v>
-      </c>
-      <c r="E45" s="6">
-        <v>64</v>
-      </c>
-      <c r="F45" s="6">
-        <v>2</v>
-      </c>
-      <c r="G45" s="20">
-        <v>0</v>
-      </c>
-      <c r="H45" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+      <c r="I46" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
         <v>128</v>
       </c>
-      <c r="I45" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
-      </c>
-      <c r="J45" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="6">
-        <v>4</v>
-      </c>
-      <c r="E46" s="6">
+      <c r="J46" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K46" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="14">
+        <v>4</v>
+      </c>
+      <c r="E47" s="14">
+        <v>256</v>
+      </c>
+      <c r="F47" s="14">
+        <v>1</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0</v>
+      </c>
+      <c r="H47" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>256</v>
+      </c>
+      <c r="I47" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>256</v>
+      </c>
+      <c r="J47" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K47" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="14">
+        <v>1</v>
+      </c>
+      <c r="E48" s="14">
+        <v>1</v>
+      </c>
+      <c r="F48" s="14">
+        <v>2</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0</v>
+      </c>
+      <c r="H48" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>2</v>
+      </c>
+      <c r="I48" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>2</v>
+      </c>
+      <c r="J48" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>2</v>
+      </c>
+      <c r="K48" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="14">
+        <v>1</v>
+      </c>
+      <c r="E49" s="14">
+        <v>1</v>
+      </c>
+      <c r="F49" s="14">
+        <v>4</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0</v>
+      </c>
+      <c r="H49" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>4</v>
+      </c>
+      <c r="I49" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>4</v>
+      </c>
+      <c r="J49" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>4</v>
+      </c>
+      <c r="K49" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="15">
+        <v>1</v>
+      </c>
+      <c r="E50" s="15">
+        <v>1</v>
+      </c>
+      <c r="F50" s="15">
+        <v>8</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0</v>
+      </c>
+      <c r="H50" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>8</v>
+      </c>
+      <c r="I50" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>8</v>
+      </c>
+      <c r="J50" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="K50" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="15">
+        <v>1</v>
+      </c>
+      <c r="E51" s="15">
+        <v>1</v>
+      </c>
+      <c r="F51" s="15">
+        <v>16</v>
+      </c>
+      <c r="G51" s="9">
+        <v>0</v>
+      </c>
+      <c r="H51" s="10">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>16</v>
+      </c>
+      <c r="I51" s="10">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>16</v>
+      </c>
+      <c r="J51" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="K51" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="15">
+        <v>1</v>
+      </c>
+      <c r="E52" s="15">
+        <v>1</v>
+      </c>
+      <c r="F52" s="15">
         <v>32</v>
       </c>
-      <c r="F46" s="6">
-        <v>1</v>
-      </c>
-      <c r="G46" s="6">
+      <c r="G52" s="9">
+        <v>0</v>
+      </c>
+      <c r="H52" s="10">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
         <v>32</v>
       </c>
-      <c r="H46" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+      <c r="I52" s="10">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
         <v>32</v>
       </c>
-      <c r="I46" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+      <c r="J52" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>32</v>
       </c>
-      <c r="J46" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="14">
-        <v>4</v>
-      </c>
-      <c r="E47" s="14">
+      <c r="K52" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="14">
+        <v>1</v>
+      </c>
+      <c r="E53" s="15">
+        <v>1</v>
+      </c>
+      <c r="F53" s="15">
+        <v>64</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0</v>
+      </c>
+      <c r="H53" s="10">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>64</v>
+      </c>
+      <c r="I53" s="10">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>64</v>
+      </c>
+      <c r="J53" s="11">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="K53" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="14">
-        <v>16</v>
-      </c>
-      <c r="G47" s="6">
-        <v>0</v>
-      </c>
-      <c r="H47" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>256</v>
-      </c>
-      <c r="I47" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>256</v>
-      </c>
-      <c r="J47" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="14">
-        <v>4</v>
-      </c>
-      <c r="E48" s="14">
-        <v>8</v>
-      </c>
-      <c r="F48" s="14">
-        <v>32</v>
-      </c>
-      <c r="G48" s="6">
-        <v>0</v>
-      </c>
-      <c r="H48" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>256</v>
-      </c>
-      <c r="I48" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>256</v>
-      </c>
-      <c r="J48" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="14">
-        <v>4</v>
-      </c>
-      <c r="E49" s="14">
-        <v>4</v>
-      </c>
-      <c r="F49" s="14">
-        <v>64</v>
-      </c>
-      <c r="G49" s="6">
-        <v>0</v>
-      </c>
-      <c r="H49" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>256</v>
-      </c>
-      <c r="I49" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>256</v>
-      </c>
-      <c r="J49" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="14">
-        <v>4</v>
-      </c>
-      <c r="E50" s="14">
-        <v>2</v>
-      </c>
-      <c r="F50" s="14">
-        <v>128</v>
-      </c>
-      <c r="G50" s="6">
-        <v>0</v>
-      </c>
-      <c r="H50" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>256</v>
-      </c>
-      <c r="I50" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>256</v>
-      </c>
-      <c r="J50" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="15">
-        <v>4</v>
-      </c>
-      <c r="E51" s="15">
-        <v>256</v>
-      </c>
-      <c r="F51" s="15">
-        <v>1</v>
-      </c>
-      <c r="G51" s="6">
-        <v>0</v>
-      </c>
-      <c r="H51" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>256</v>
-      </c>
-      <c r="I51" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>256</v>
-      </c>
-      <c r="J51" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="15">
-        <v>4</v>
-      </c>
-      <c r="E52" s="9">
-        <v>32</v>
-      </c>
-      <c r="F52" s="9">
-        <v>8</v>
-      </c>
-      <c r="G52" s="9">
-        <v>0</v>
-      </c>
-      <c r="H52" s="10">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>256</v>
-      </c>
-      <c r="I52" s="10">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>256</v>
-      </c>
-      <c r="J52" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="15">
-        <v>4</v>
-      </c>
-      <c r="E53" s="9">
-        <v>64</v>
-      </c>
-      <c r="F53" s="9">
-        <v>4</v>
-      </c>
-      <c r="G53" s="9">
-        <v>0</v>
-      </c>
-      <c r="H53" s="10">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>256</v>
-      </c>
-      <c r="I53" s="10">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>256</v>
-      </c>
-      <c r="J53" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="D54" s="14">
-        <v>4</v>
-      </c>
-      <c r="E54" s="9">
-        <v>128</v>
-      </c>
-      <c r="F54" s="9">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E54" s="15">
+        <v>1</v>
+      </c>
+      <c r="F54" s="15">
+        <v>1</v>
       </c>
       <c r="G54" s="6">
         <v>0</v>
       </c>
       <c r="H54" s="10">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="I54" s="10">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="J54" s="11">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D55" s="6">
-        <v>8</v>
-      </c>
-      <c r="E55" s="9">
-        <v>64</v>
-      </c>
-      <c r="F55" s="9">
-        <v>1</v>
-      </c>
-      <c r="G55" s="6">
-        <v>64</v>
-      </c>
-      <c r="H55" s="10">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>64</v>
-      </c>
-      <c r="I55" s="10">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>64</v>
-      </c>
-      <c r="J55" s="11">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="K54" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>